<commit_message>
travis install without cwb
</commit_message>
<xml_diff>
--- a/uml/partition2subcorpus.xlsx
+++ b/uml/partition2subcorpus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreasblaette/Lab/github/polmineR/uml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E4B516-7332-E845-B7D5-FE9F68C80D1F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640ED432-56D9-6D4B-BCFF-3FA85CD9395A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{E13186DF-57CC-1E4B-BA3E-3AD8063B1E08}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="58">
   <si>
     <t>as.markdown</t>
   </si>
@@ -586,7 +586,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -933,7 +933,7 @@
         <v>41</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -944,12 +944,15 @@
         <v>55</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
methods for subcorpus-class implemented/checked
</commit_message>
<xml_diff>
--- a/uml/partition2subcorpus.xlsx
+++ b/uml/partition2subcorpus.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreasblaette/Lab/github/polmineR/uml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62A80A1-3EF2-5E4A-B004-D273FEDA4D24}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84984FA4-1A9D-1448-A518-11FFFB579127}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{E13186DF-57CC-1E4B-BA3E-3AD8063B1E08}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{E13186DF-57CC-1E4B-BA3E-3AD8063B1E08}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="subcorpus_bundle" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="83">
   <si>
     <t>as.markdown</t>
   </si>
@@ -199,6 +200,81 @@
   </si>
   <si>
     <t>nein, as(x, "subcorpus")</t>
+  </si>
+  <si>
+    <t>as.DocumentTermMatrix</t>
+  </si>
+  <si>
+    <t>as.TermDocumentMatrix</t>
+  </si>
+  <si>
+    <t>as.Vcorpus</t>
+  </si>
+  <si>
+    <t>barplot</t>
+  </si>
+  <si>
+    <t>coerce</t>
+  </si>
+  <si>
+    <t>merge</t>
+  </si>
+  <si>
+    <t>summary</t>
+  </si>
+  <si>
+    <t>partition_bundle-method</t>
+  </si>
+  <si>
+    <t>bundle-method</t>
+  </si>
+  <si>
+    <t>count_bundle-method</t>
+  </si>
+  <si>
+    <t>weigh</t>
+  </si>
+  <si>
+    <t>subcorpus_bundle-method</t>
+  </si>
+  <si>
+    <t>implementiert und dokumentiert</t>
+  </si>
+  <si>
+    <t>qua Vererbung verfügbar</t>
+  </si>
+  <si>
+    <t>qua Vererbung von partition_bundle verfügbar</t>
+  </si>
+  <si>
+    <t>nicht implementiert - use case unklar!</t>
+  </si>
+  <si>
+    <t>qua Vererbung von partition_bundle</t>
+  </si>
+  <si>
+    <t>nicht sinnvoll! (weil kein stat-slot der zu befüllen wäre)</t>
+  </si>
+  <si>
+    <t>Umweg über count_bundle</t>
+  </si>
+  <si>
+    <t>erbt von partition_bundle, aber Tabellenspalte "partition"</t>
+  </si>
+  <si>
+    <t>geerbt von partition_bundle, aber noch nicht ideal, siehe issue #76</t>
+  </si>
+  <si>
+    <t>inherited from partition_bundle</t>
+  </si>
+  <si>
+    <t>eigens implementiert</t>
+  </si>
+  <si>
+    <t>geerbt von partition_bundle</t>
+  </si>
+  <si>
+    <t>defined for subcorpus_bundle</t>
   </si>
 </sst>
 </file>
@@ -240,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -258,6 +334,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -579,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF67A48-85E9-334B-B073-14C5F5E7B53F}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -776,11 +855,11 @@
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
       <c r="F12" s="1" t="s">
         <v>45</v>
       </c>
@@ -789,11 +868,11 @@
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
       <c r="F13" s="1" t="s">
         <v>43</v>
       </c>
@@ -1041,4 +1120,262 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CA5236-E0EF-3A48-9839-8444A42013B5}">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
label-method for kwic working
</commit_message>
<xml_diff>
--- a/uml/partition2subcorpus.xlsx
+++ b/uml/partition2subcorpus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreasblaette/Lab/github/polmineR/uml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84984FA4-1A9D-1448-A518-11FFFB579127}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765096FC-DC4E-1545-ADE9-A9CC291B07BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{E13186DF-57CC-1E4B-BA3E-3AD8063B1E08}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="86">
   <si>
     <t>as.markdown</t>
   </si>
@@ -268,13 +268,22 @@
     <t>inherited from partition_bundle</t>
   </si>
   <si>
-    <t>eigens implementiert</t>
-  </si>
-  <si>
     <t>geerbt von partition_bundle</t>
   </si>
   <si>
     <t>defined for subcorpus_bundle</t>
+  </si>
+  <si>
+    <t>inherited from count_bundle</t>
+  </si>
+  <si>
+    <t>implemented explicitly for subcorpus_bundle</t>
+  </si>
+  <si>
+    <t>implemented explicitly</t>
+  </si>
+  <si>
+    <t>[not applicable]</t>
   </si>
 </sst>
 </file>
@@ -1127,7 +1136,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1210,6 +1219,9 @@
       <c r="B6" s="7" t="s">
         <v>30</v>
       </c>
+      <c r="E6" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1276,6 +1288,9 @@
       <c r="D12" t="s">
         <v>30</v>
       </c>
+      <c r="E12" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1326,7 +1341,7 @@
         <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1344,6 +1359,9 @@
       <c r="B19" s="7" t="s">
         <v>30</v>
       </c>
+      <c r="E19" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -1353,7 +1371,7 @@
         <v>30</v>
       </c>
       <c r="E20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1364,7 +1382,7 @@
         <v>30</v>
       </c>
       <c r="E21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1373,6 +1391,9 @@
       </c>
       <c r="D22" s="7" t="s">
         <v>30</v>
+      </c>
+      <c r="E22" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>